<commit_message>
Update for the final release on master
</commit_message>
<xml_diff>
--- a/src/main/resources/documentation/TCO.xlsx
+++ b/src/main/resources/documentation/TCO.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Uni\US2\US\PSG2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40019_{8C19D485-C334-495D-8767-8C4023B3A98B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76919AE-FF06-48E4-87EA-F3D443A3CABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TCO Calculator" sheetId="1" r:id="rId1"/>
     <sheet name="TCO Chart" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'TCO Calculator'!$A$1:$G$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'TCO Calculator'!$A$1:$G$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
   <si>
     <t>CI</t>
   </si>
@@ -200,16 +200,22 @@
   </si>
   <si>
     <t>Coste total de operación G2-24</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>SonarCloud</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -430,7 +436,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -441,7 +447,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -510,19 +516,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -534,10 +527,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -547,6 +540,19 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1154,7 +1160,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Chart2">
     <tabColor indexed="18"/>
   </sheetPr>
@@ -1172,7 +1178,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8583448" cy="5846379"/>
+    <xdr:ext cx="8558893" cy="5823857"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -1497,24 +1503,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="57"/>
   </sheetPr>
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" customWidth="1"/>
@@ -1522,36 +1528,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="30"/>
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="15"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
       <c r="F3" s="15"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="22" t="s">
         <v>48</v>
       </c>
@@ -1566,7 +1572,7 @@
       <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="16" t="s">
         <v>49</v>
       </c>
@@ -1583,24 +1589,24 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="13">
-        <f>C51+D85</f>
-        <v>27143</v>
+        <f>C53+D89</f>
+        <v>27386.799999999999</v>
       </c>
       <c r="D6" s="13">
-        <f>C64+D85</f>
-        <v>27171</v>
+        <f>C68+D89</f>
+        <v>27414.799999999999</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="16" t="s">
         <v>50</v>
       </c>
@@ -1617,14 +1623,14 @@
       <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="38">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="38">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="E8" s="13"/>
@@ -1632,14 +1638,14 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="39">
         <v>10000</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="39">
         <v>40000</v>
       </c>
       <c r="E9" s="13"/>
@@ -1647,11 +1653,11 @@
       <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="43" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="23"/>
@@ -1660,7 +1666,7 @@
       <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="22" t="s">
         <v>47</v>
       </c>
@@ -1677,7 +1683,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="16">
         <v>0</v>
       </c>
@@ -1697,7 +1703,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="16">
         <v>5000</v>
       </c>
@@ -1717,7 +1723,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="16">
         <v>10000</v>
       </c>
@@ -1737,7 +1743,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="16">
         <v>15000</v>
       </c>
@@ -1757,7 +1763,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="16">
         <v>20000</v>
       </c>
@@ -1777,7 +1783,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="16">
         <v>25000</v>
       </c>
@@ -1797,7 +1803,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="31"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="16">
         <v>30000</v>
       </c>
@@ -1817,7 +1823,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="16">
         <v>35000</v>
       </c>
@@ -1837,7 +1843,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="16">
         <v>40000</v>
       </c>
@@ -1857,7 +1863,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="16">
         <v>45000</v>
       </c>
@@ -1877,7 +1883,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="16">
         <v>50000</v>
       </c>
@@ -1897,7 +1903,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="16">
         <v>55000</v>
       </c>
@@ -1917,11 +1923,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="11"/>
       <c r="G24" s="3"/>
     </row>
@@ -2114,10 +2120,10 @@
     </row>
     <row r="38" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="35">
+      <c r="C38" s="31">
         <f>SUM(C27:C37)</f>
         <v>4142</v>
       </c>
@@ -2138,7 +2144,7 @@
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="31"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="24" t="s">
         <v>40</v>
       </c>
@@ -2151,7 +2157,7 @@
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="31"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="20" t="s">
         <v>17</v>
       </c>
@@ -2164,7 +2170,7 @@
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="31"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="20" t="s">
         <v>18</v>
       </c>
@@ -2177,12 +2183,12 @@
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="31"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C43" s="6">
-        <v>16</v>
+        <v>3.28</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>13</v>
@@ -2190,7 +2196,7 @@
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="31"/>
+      <c r="A44" s="47"/>
       <c r="B44" s="20" t="s">
         <v>20</v>
       </c>
@@ -2203,145 +2209,149 @@
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="31"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="6">
+        <v>10</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="47"/>
+      <c r="B46" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="47"/>
+      <c r="B47" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C47" s="7">
         <v>0</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="5"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="31"/>
-      <c r="B46" s="20" t="s">
+      <c r="D47" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="47"/>
+      <c r="B48" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C48" s="7">
         <v>0</v>
       </c>
-      <c r="D46" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="31"/>
-      <c r="B47" s="20" t="s">
+      <c r="D48" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="47"/>
+      <c r="B49" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="8">
-        <v>70</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="31"/>
-      <c r="B48" s="20" t="s">
+      <c r="C49" s="8">
+        <v>345</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="47"/>
+      <c r="B50" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C50" s="8">
+        <v>10</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="47"/>
+      <c r="B51" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="8">
+        <v>6.52</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="47"/>
+      <c r="B52" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="6">
+        <v>12</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="31">
+        <f>SUM(C41:C52)</f>
+        <v>386.79999999999995</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="31"/>
-      <c r="B49" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" s="8">
-        <v>0</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="31"/>
-      <c r="B50" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="6">
-        <v>12</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="35">
-        <f>SUM(C41:C50)</f>
-        <v>143</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D53" s="26" t="s">
+      <c r="D55" s="26" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="6">
-        <v>0</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C55" s="6">
-        <v>0</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B56" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C56" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B57" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C57" s="6">
         <v>0</v>
@@ -2352,43 +2362,43 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B58" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" s="7">
+        <v>19</v>
+      </c>
+      <c r="C58" s="6">
+        <v>3.28</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="6">
         <v>0</v>
       </c>
-      <c r="D58" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B59" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="7">
+      <c r="D59" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="6">
+        <v>10</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="6">
         <v>0</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B60" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" s="8">
-        <v>70</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61" s="8">
-        <v>45</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>13</v>
@@ -2396,9 +2406,9 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B62" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="8">
+        <v>21</v>
+      </c>
+      <c r="C62" s="7">
         <v>0</v>
       </c>
       <c r="D62" s="18" t="s">
@@ -2407,117 +2417,101 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B63" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B64" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C64" s="8">
+        <v>345</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="8">
+        <v>10</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="8">
+        <v>6.52</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C63" s="6">
+      <c r="C67" s="6">
         <v>40</v>
       </c>
-      <c r="D63" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="36" t="s">
+      <c r="D67" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C64" s="35">
-        <f>SUM(C54:C63)</f>
-        <v>171</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B66" s="24" t="s">
+      <c r="C68" s="31">
+        <f>SUM(C56:C67)</f>
+        <v>414.79999999999995</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="44"/>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B67" s="29" t="s">
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="40"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="37" t="s">
+      <c r="C71" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D67" s="37" t="s">
+      <c r="D71" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E67" s="38" t="s">
+      <c r="E71" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F67" s="46"/>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D68" s="6">
-        <v>1800</v>
-      </c>
-      <c r="E68" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F68" s="12"/>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B69" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D69" s="6">
-        <v>1800</v>
-      </c>
-      <c r="E69" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F69" s="12"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D70" s="6">
-        <v>1800</v>
-      </c>
-      <c r="E70" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F70" s="12"/>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C71" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D71" s="6">
-        <v>1800</v>
-      </c>
-      <c r="E71" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="12"/>
+      <c r="F71" s="42"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C72" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" s="35" t="s">
         <v>37</v>
       </c>
       <c r="D72" s="6">
@@ -2529,20 +2523,26 @@
       <c r="F72" s="12"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B73" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C73" s="27"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="45"/>
+      <c r="B73" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C73" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73" s="6">
+        <v>1800</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="12"/>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B74" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C74" s="39" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C74" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="D74" s="6">
         <v>1800</v>
@@ -2554,9 +2554,9 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B75" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C75" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C75" s="35" t="s">
         <v>37</v>
       </c>
       <c r="D75" s="6">
@@ -2569,10 +2569,10 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B76" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C76" s="39" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="C76" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="D76" s="6">
         <v>1800</v>
@@ -2583,25 +2583,19 @@
       <c r="F76" s="12"/>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B77" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C77" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D77" s="6">
-        <v>1800</v>
-      </c>
-      <c r="E77" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="12"/>
+      <c r="B77" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" s="27"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="41"/>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B78" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C78" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" s="35" t="s">
         <v>37</v>
       </c>
       <c r="D78" s="6">
@@ -2613,20 +2607,26 @@
       <c r="F78" s="12"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B79" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C79" s="27"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="45"/>
+      <c r="B79" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" s="6">
+        <v>1800</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="12"/>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B80" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" s="39" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C80" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="D80" s="6">
         <v>1800</v>
@@ -2638,9 +2638,9 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B81" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C81" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="35" t="s">
         <v>37</v>
       </c>
       <c r="D81" s="6">
@@ -2653,10 +2653,10 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B82" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C82" s="39" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="C82" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="D82" s="6">
         <v>1800</v>
@@ -2667,25 +2667,19 @@
       <c r="F82" s="12"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B83" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C83" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D83" s="6">
-        <v>1800</v>
-      </c>
-      <c r="E83" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F83" s="12"/>
+      <c r="B83" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C83" s="27"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="41"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C84" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="35" t="s">
         <v>37</v>
       </c>
       <c r="D84" s="6">
@@ -2696,19 +2690,79 @@
       </c>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="36" t="s">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B85" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D85" s="6">
+        <v>1800</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="12"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B86" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C86" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D86" s="6">
+        <v>1800</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="12"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C87" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D87" s="6">
+        <v>1800</v>
+      </c>
+      <c r="E87" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="12"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B88" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C88" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D88" s="6">
+        <v>1800</v>
+      </c>
+      <c r="E88" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F88" s="12"/>
+    </row>
+    <row r="89" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C85" s="41"/>
-      <c r="D85" s="40">
-        <f>SUM(D68:D84)</f>
+      <c r="C89" s="37"/>
+      <c r="D89" s="36">
+        <f>SUM(D72:D88)</f>
         <v>27000</v>
       </c>
-      <c r="E85" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F85" s="12"/>
+      <c r="E89" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2716,7 +2770,7 @@
     <mergeCell ref="A2:E3"/>
     <mergeCell ref="A24:E24"/>
     <mergeCell ref="A4:A23"/>
-    <mergeCell ref="A40:A50"/>
+    <mergeCell ref="A40:A52"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="1.18" right="0.75" top="0.81" bottom="0.17" header="0.18" footer="0.17"/>

</xml_diff>